<commit_message>
correct function to rename columns.
</commit_message>
<xml_diff>
--- a/data training/suivi gainz (1).xlsx
+++ b/data training/suivi gainz (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander.maclennan/Documents/Dev Projects/Workout Analysis/data training/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1C7D9-B10A-A44D-864A-945C8976FAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11025F8D-AF1A-FE4C-BDD3-71BDEDFF0168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16915,7 +16915,7 @@
   <dimension ref="A1:AF27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH9" sqref="AH9"/>
+      <selection activeCell="C3" sqref="C3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>